<commit_message>
Company Name is in report
</commit_message>
<xml_diff>
--- a/Screener/Fundamental_Info.xlsx
+++ b/Screener/Fundamental_Info.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhill24\Desktop\Financial-Advisor-Senior-Project-master\Screener\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse\Desktop\Financial-Advisor-Senior-Project\Screener\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218A0822-358C-4F3B-92EA-4C1BBF312B3D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="5535" yWindow="0" windowWidth="15000" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Basic</t>
   </si>
@@ -68,13 +69,13 @@
     <t xml:space="preserve">Price to earnings is just one number to look at. High price to earnings can mean that the company is overvalued or it means that </t>
   </si>
   <si>
-    <t>justatest</t>
+    <t>name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -385,16 +386,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -411,7 +412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -422,7 +423,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -433,7 +434,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -444,7 +445,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>

</xml_diff>